<commit_message>
scriviamo risultato su file
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13515" windowHeight="7095" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13515" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Waters" sheetId="1" r:id="rId1"/>
     <sheet name="Salts" sheetId="2" r:id="rId2"/>
     <sheet name="Target" sheetId="3" r:id="rId3"/>
-    <sheet name="Recipe" sheetId="4" r:id="rId4"/>
+    <sheet name="Recipe" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
@@ -457,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1157,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Localized all the messages and the output files
I kept the sheet names but added a prefix to avoid problems loading
xlsx created with a different locale: U# for sheets the user is supposed
to edit, R for the result/recipe sheet and D# for registry profiles
sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/input.xlsx
+++ b/src/test/resources/input.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alessio\Progetti\personal\rabdomante\target\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alessio\Progetti\personal\rabdomante\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Acque Disponibili" sheetId="1" r:id="rId1"/>
-    <sheet name="Sali" sheetId="2" r:id="rId2"/>
-    <sheet name="Obiettivo" sheetId="3" r:id="rId3"/>
-    <sheet name="Acque Commerciali" sheetId="5" r:id="rId4"/>
-    <sheet name="Ricetta" sheetId="6" r:id="rId5"/>
+    <sheet name="U1. Acque Disponibili" sheetId="1" r:id="rId1"/>
+    <sheet name="U2. Sali" sheetId="2" r:id="rId2"/>
+    <sheet name="U3. Obiettivo" sheetId="3" r:id="rId3"/>
+    <sheet name="D1. Acque Commerciali" sheetId="5" r:id="rId4"/>
+    <sheet name="R. Ricetta" sheetId="6" r:id="rId5"/>
+    <sheet name="D2. Profili Comuni" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
 </workbook>
@@ -14767,8 +14768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14785,4 +14786,18 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>